<commit_message>
add res boundary attack for SEED 0
</commit_message>
<xml_diff>
--- a/results/SEED_0/result.xlsx
+++ b/results/SEED_0/result.xlsx
@@ -803,88 +803,88 @@
         <v>5.46418285369873</v>
       </c>
       <c r="D4" t="n">
-        <v>5.116778373718262</v>
+        <v>5.116774082183838</v>
       </c>
       <c r="E4" t="n">
-        <v>5.253917997533625</v>
+        <v>5.253917217254639</v>
       </c>
       <c r="F4" t="n">
-        <v>5.095665975050493</v>
+        <v>5.095665801655162</v>
       </c>
       <c r="G4" t="n">
-        <v>4.991347009485418</v>
+        <v>4.99134670604359</v>
       </c>
       <c r="H4" t="n">
-        <v>4.966341929002241</v>
+        <v>4.966341798955744</v>
       </c>
       <c r="I4" t="n">
-        <v>5.025414185090498</v>
+        <v>5.025414076718417</v>
       </c>
       <c r="J4" t="n">
-        <v>5.448878331617876</v>
+        <v>5.448877919803966</v>
       </c>
       <c r="K4" t="n">
-        <v>6.088291601701216</v>
+        <v>6.088291189887307</v>
       </c>
       <c r="L4" t="n">
-        <v>9.670856454155661</v>
+        <v>9.670856389132412</v>
       </c>
       <c r="M4" t="n">
-        <v>5.487316738475453</v>
+        <v>5.487314961173317</v>
       </c>
       <c r="N4" t="n">
-        <v>5.51210355758667</v>
+        <v>5.512102994051847</v>
       </c>
       <c r="O4" t="n">
-        <v>5.537866115570068</v>
+        <v>5.537866158918901</v>
       </c>
       <c r="P4" t="n">
-        <v>5.56558860432018</v>
+        <v>5.565588300878352</v>
       </c>
       <c r="Q4" t="n">
-        <v>5.596527229655873</v>
+        <v>5.596526622772217</v>
       </c>
       <c r="R4" t="n">
-        <v>5.692193334752863</v>
+        <v>5.692192337729714</v>
       </c>
       <c r="S4" t="n">
-        <v>5.830752719532359</v>
+        <v>5.830752155997536</v>
       </c>
       <c r="T4" t="n">
-        <v>6.882791996002197</v>
+        <v>6.882790955630216</v>
       </c>
       <c r="U4" t="n">
-        <v>5.487316738475453</v>
+        <v>5.487314961173317</v>
       </c>
       <c r="V4" t="n">
-        <v>5.51733381097967</v>
+        <v>5.517332900654186</v>
       </c>
       <c r="W4" t="n">
-        <v>5.557119759646329</v>
+        <v>5.557119022716176</v>
       </c>
       <c r="X4" t="n">
-        <v>5.6156925721602</v>
+        <v>5.61569205197421</v>
       </c>
       <c r="Y4" t="n">
-        <v>5.68837933106856</v>
+        <v>5.688378810882568</v>
       </c>
       <c r="Z4" t="n">
-        <v>5.895527883009477</v>
+        <v>5.895527276125821</v>
       </c>
       <c r="AA4" t="n">
-        <v>6.406144532290372</v>
+        <v>6.406144272197377</v>
       </c>
       <c r="AB4" t="n">
-        <v>9.406350786035711</v>
+        <v>9.40635015747764</v>
       </c>
       <c r="AC4" t="n">
-        <v>6.633081436157227</v>
+        <v>6.633080005645752</v>
       </c>
       <c r="AD4" t="n">
-        <v>7.9528489112854</v>
+        <v>7.952848434448242</v>
       </c>
       <c r="AE4" t="n">
-        <v>9.358843803405762</v>
+        <v>9.358842849731445</v>
       </c>
       <c r="AF4" t="n">
         <v>10.77638912200928</v>
@@ -896,13 +896,13 @@
         <v>15.7540979385376</v>
       </c>
       <c r="AI4" t="n">
-        <v>19.31417846679688</v>
+        <v>19.31417655944824</v>
       </c>
       <c r="AJ4" t="n">
         <v>33.50799942016602</v>
       </c>
       <c r="AK4" t="n">
-        <v>6.896324634552002</v>
+        <v>6.896325588226318</v>
       </c>
       <c r="AL4" t="n">
         <v>8.332001686096191</v>
@@ -914,7 +914,7 @@
         <v>11.21237087249756</v>
       </c>
       <c r="AO4" t="n">
-        <v>12.6558084487915</v>
+        <v>12.65580654144287</v>
       </c>
       <c r="AP4" t="n">
         <v>16.26960754394531</v>
@@ -923,7 +923,7 @@
         <v>19.88080406188965</v>
       </c>
       <c r="AR4" t="n">
-        <v>34.203125</v>
+        <v>34.20312118530273</v>
       </c>
     </row>
     <row r="5">
@@ -934,130 +934,130 @@
         </is>
       </c>
       <c r="C5" t="n">
-        <v>6.734641793402914</v>
+        <v>6.734641510188345</v>
       </c>
       <c r="D5" t="n">
-        <v>6.450305830927709</v>
+        <v>6.450301099742845</v>
       </c>
       <c r="E5" t="n">
-        <v>6.527816887116773</v>
+        <v>6.527815741245532</v>
       </c>
       <c r="F5" t="n">
-        <v>6.377900731569802</v>
+        <v>6.377900519117718</v>
       </c>
       <c r="G5" t="n">
-        <v>6.287256204465764</v>
+        <v>6.287255692742543</v>
       </c>
       <c r="H5" t="n">
-        <v>6.261524267992148</v>
+        <v>6.261524071527155</v>
       </c>
       <c r="I5" t="n">
-        <v>6.302449074530021</v>
+        <v>6.302448558058922</v>
       </c>
       <c r="J5" t="n">
-        <v>6.684886065713416</v>
+        <v>6.684885841711952</v>
       </c>
       <c r="K5" t="n">
-        <v>7.431644669110743</v>
+        <v>7.431644433685793</v>
       </c>
       <c r="L5" t="n">
-        <v>12.14983075625002</v>
+        <v>12.14983024173297</v>
       </c>
       <c r="M5" t="n">
-        <v>6.766257874887638</v>
+        <v>6.76625605139643</v>
       </c>
       <c r="N5" t="n">
-        <v>6.800092876969968</v>
+        <v>6.80009246083984</v>
       </c>
       <c r="O5" t="n">
-        <v>6.836268265415818</v>
+        <v>6.836267776171312</v>
       </c>
       <c r="P5" t="n">
-        <v>6.876502213009205</v>
+        <v>6.876501999081554</v>
       </c>
       <c r="Q5" t="n">
-        <v>6.922413426641596</v>
+        <v>6.92241316543147</v>
       </c>
       <c r="R5" t="n">
-        <v>7.063611180060683</v>
+        <v>7.063610369436519</v>
       </c>
       <c r="S5" t="n">
-        <v>7.282428740647886</v>
+        <v>7.282427951305918</v>
       </c>
       <c r="T5" t="n">
-        <v>8.995483916537573</v>
+        <v>8.995482678021409</v>
       </c>
       <c r="U5" t="n">
-        <v>6.766257874887638</v>
+        <v>6.76625605139643</v>
       </c>
       <c r="V5" t="n">
-        <v>6.807559030013329</v>
+        <v>6.807557923353545</v>
       </c>
       <c r="W5" t="n">
-        <v>6.8616706279941</v>
+        <v>6.86166981181509</v>
       </c>
       <c r="X5" t="n">
-        <v>6.936988834601291</v>
+        <v>6.9369883134406</v>
       </c>
       <c r="Y5" t="n">
-        <v>7.029220941255786</v>
+        <v>7.029220195650633</v>
       </c>
       <c r="Z5" t="n">
-        <v>7.286538928517171</v>
+        <v>7.28653842844994</v>
       </c>
       <c r="AA5" t="n">
-        <v>7.89815860964087</v>
+        <v>7.898158527152222</v>
       </c>
       <c r="AB5" t="n">
-        <v>11.3226680574001</v>
+        <v>11.32266739400024</v>
       </c>
       <c r="AC5" t="n">
-        <v>7.842686797651344</v>
+        <v>7.842686068048554</v>
       </c>
       <c r="AD5" t="n">
-        <v>9.038401586954981</v>
+        <v>9.038401164900559</v>
       </c>
       <c r="AE5" t="n">
         <v>10.2925862713567</v>
       </c>
       <c r="AF5" t="n">
-        <v>11.5867368971522</v>
+        <v>11.58673623869289</v>
       </c>
       <c r="AG5" t="n">
-        <v>12.90946717147409</v>
+        <v>12.90946658048187</v>
       </c>
       <c r="AH5" t="n">
-        <v>16.29623736618124</v>
+        <v>16.2962354935048</v>
       </c>
       <c r="AI5" t="n">
-        <v>19.74572321301699</v>
+        <v>19.74572244025272</v>
       </c>
       <c r="AJ5" t="n">
-        <v>33.74225533247407</v>
+        <v>33.74225171474556</v>
       </c>
       <c r="AK5" t="n">
         <v>7.929086867261828</v>
       </c>
       <c r="AL5" t="n">
-        <v>9.195819435633425</v>
+        <v>9.195818605974369</v>
       </c>
       <c r="AM5" t="n">
-        <v>10.50993313289898</v>
+        <v>10.50993276993784</v>
       </c>
       <c r="AN5" t="n">
-        <v>11.85596940870367</v>
+        <v>11.8559681216904</v>
       </c>
       <c r="AO5" t="n">
-        <v>13.22457923147687</v>
+        <v>13.22457807765644</v>
       </c>
       <c r="AP5" t="n">
-        <v>16.70772672520767</v>
+        <v>16.70772581193026</v>
       </c>
       <c r="AQ5" t="n">
-        <v>20.23496545349897</v>
+        <v>20.23496469941865</v>
       </c>
       <c r="AR5" t="n">
-        <v>34.42382541001762</v>
+        <v>34.42382363696779</v>
       </c>
     </row>
     <row r="6">
@@ -1083,16 +1083,16 @@
         <v>0.9995588064193726</v>
       </c>
       <c r="H6" t="n">
-        <v>0.9995182156562805</v>
+        <v>0.9995183348655701</v>
       </c>
       <c r="I6" t="n">
-        <v>0.9994677901268005</v>
+        <v>0.9994680285453796</v>
       </c>
       <c r="J6" t="n">
-        <v>0.9992961287498474</v>
+        <v>0.9992963075637817</v>
       </c>
       <c r="K6" t="n">
-        <v>0.999052107334137</v>
+        <v>0.9990522861480713</v>
       </c>
       <c r="L6" t="n">
         <v>0.9973534345626831</v>
@@ -1101,25 +1101,25 @@
         <v>0.9996201992034912</v>
       </c>
       <c r="N6" t="n">
-        <v>0.9996169805526733</v>
+        <v>0.9996170997619629</v>
       </c>
       <c r="O6" t="n">
-        <v>0.9996134042739868</v>
+        <v>0.9996135234832764</v>
       </c>
       <c r="P6" t="n">
-        <v>0.9996092319488525</v>
+        <v>0.999609112739563</v>
       </c>
       <c r="Q6" t="n">
-        <v>0.9996042251586914</v>
+        <v>0.9996042847633362</v>
       </c>
       <c r="R6" t="n">
-        <v>0.9995881319046021</v>
+        <v>0.9995881915092468</v>
       </c>
       <c r="S6" t="n">
-        <v>0.9995603561401367</v>
+        <v>0.9995604753494263</v>
       </c>
       <c r="T6" t="n">
-        <v>0.9992969632148743</v>
+        <v>0.9992970824241638</v>
       </c>
       <c r="U6" t="n">
         <v>0.9996201992034912</v>
@@ -1128,25 +1128,25 @@
         <v>0.9996161460876465</v>
       </c>
       <c r="W6" t="n">
-        <v>0.9996112585067749</v>
+        <v>0.9996113777160645</v>
       </c>
       <c r="X6" t="n">
-        <v>0.9996050596237183</v>
+        <v>0.9996052980422974</v>
       </c>
       <c r="Y6" t="n">
         <v>0.9995982050895691</v>
       </c>
       <c r="Z6" t="n">
-        <v>0.999580979347229</v>
+        <v>0.9995810985565186</v>
       </c>
       <c r="AA6" t="n">
-        <v>0.9995374083518982</v>
+        <v>0.9995375871658325</v>
       </c>
       <c r="AB6" t="n">
-        <v>0.9992917776107788</v>
+        <v>0.9992920160293579</v>
       </c>
       <c r="AC6" t="n">
-        <v>0.9995917081832886</v>
+        <v>0.9995918273925781</v>
       </c>
       <c r="AD6" t="n">
         <v>0.9995480179786682</v>
@@ -1155,7 +1155,7 @@
         <v>0.9994911551475525</v>
       </c>
       <c r="AF6" t="n">
-        <v>0.9994204044342041</v>
+        <v>0.9994205236434937</v>
       </c>
       <c r="AG6" t="n">
         <v>0.9993354082107544</v>
@@ -1167,22 +1167,22 @@
         <v>0.9986723661422729</v>
       </c>
       <c r="AJ6" t="n">
-        <v>0.9958337545394897</v>
+        <v>0.9958338141441345</v>
       </c>
       <c r="AK6" t="n">
-        <v>0.9994995594024658</v>
+        <v>0.9994996786117554</v>
       </c>
       <c r="AL6" t="n">
         <v>0.9993337392807007</v>
       </c>
       <c r="AM6" t="n">
-        <v>0.9991234540939331</v>
+        <v>0.9991235733032227</v>
       </c>
       <c r="AN6" t="n">
-        <v>0.9988675117492676</v>
+        <v>0.9988676905632019</v>
       </c>
       <c r="AO6" t="n">
-        <v>0.9985643029212952</v>
+        <v>0.9985643625259399</v>
       </c>
       <c r="AP6" t="n">
         <v>0.9975900053977966</v>
@@ -1191,7 +1191,7 @@
         <v>0.9962887763977051</v>
       </c>
       <c r="AR6" t="n">
-        <v>0.9874228835105896</v>
+        <v>0.9874229431152344</v>
       </c>
     </row>
     <row r="7">
@@ -1206,94 +1206,94 @@
         </is>
       </c>
       <c r="C7" t="n">
-        <v>3.097177028656006</v>
+        <v>3.097176313400269</v>
       </c>
       <c r="D7" t="n">
-        <v>2.733250141143799</v>
+        <v>2.733249664306641</v>
       </c>
       <c r="E7" t="n">
-        <v>2.78155838359486</v>
+        <v>2.781556736339222</v>
       </c>
       <c r="F7" t="n">
-        <v>2.979455232620239</v>
+        <v>2.979454582387751</v>
       </c>
       <c r="G7" t="n">
-        <v>3.622935381802646</v>
+        <v>3.622937029058283</v>
       </c>
       <c r="H7" t="n">
-        <v>4.608063892884688</v>
+        <v>4.608065518465909</v>
       </c>
       <c r="I7" t="n">
-        <v>5.808242537758567</v>
+        <v>5.808245073665272</v>
       </c>
       <c r="J7" t="n">
-        <v>9.072190848263828</v>
+        <v>9.072193600914694</v>
       </c>
       <c r="K7" t="n">
-        <v>12.37476706504822</v>
+        <v>12.37477133490822</v>
       </c>
       <c r="L7" t="n">
-        <v>24.55263029445301</v>
+        <v>24.55263458598744</v>
       </c>
       <c r="M7" t="n">
-        <v>3.020496108315208</v>
+        <v>3.020493637431751</v>
       </c>
       <c r="N7" t="n">
-        <v>2.963758165186102</v>
+        <v>2.963756041093306</v>
       </c>
       <c r="O7" t="n">
-        <v>2.916305065155029</v>
+        <v>2.916302637620406</v>
       </c>
       <c r="P7" t="n">
-        <v>2.882257808338512</v>
+        <v>2.882255900989879</v>
       </c>
       <c r="Q7" t="n">
-        <v>2.872651533647017</v>
+        <v>2.872648846019398</v>
       </c>
       <c r="R7" t="n">
-        <v>2.96236328645186</v>
+        <v>2.962361465800892</v>
       </c>
       <c r="S7" t="n">
-        <v>3.223326726393266</v>
+        <v>3.223325425928289</v>
       </c>
       <c r="T7" t="n">
-        <v>5.074632146141746</v>
+        <v>5.074631625955755</v>
       </c>
       <c r="U7" t="n">
-        <v>2.78155838359486</v>
+        <v>2.781556736339222</v>
       </c>
       <c r="V7" t="n">
-        <v>2.978997794064608</v>
+        <v>2.978997165506536</v>
       </c>
       <c r="W7" t="n">
-        <v>3.620043624531139</v>
+        <v>3.620044968344949</v>
       </c>
       <c r="X7" t="n">
-        <v>4.60312522541393</v>
+        <v>4.603126655925404</v>
       </c>
       <c r="Y7" t="n">
-        <v>5.797100934115323</v>
+        <v>5.797103448347612</v>
       </c>
       <c r="Z7" t="n">
-        <v>8.374000896107066</v>
+        <v>8.374004754153164</v>
       </c>
       <c r="AA7" t="n">
-        <v>12.21166461164301</v>
+        <v>12.21166714754972</v>
       </c>
       <c r="AB7" t="n">
-        <v>23.19226267121055</v>
+        <v>23.19226791641929</v>
       </c>
       <c r="AC7" t="n">
-        <v>4.313810348510742</v>
+        <v>4.313807964324951</v>
       </c>
       <c r="AD7" t="n">
-        <v>5.673810958862305</v>
+        <v>5.673808574676514</v>
       </c>
       <c r="AE7" t="n">
-        <v>7.05316162109375</v>
+        <v>7.053157329559326</v>
       </c>
       <c r="AF7" t="n">
-        <v>8.44214916229248</v>
+        <v>8.442146301269531</v>
       </c>
       <c r="AG7" t="n">
         <v>9.839560508728027</v>
@@ -1302,28 +1302,28 @@
         <v>13.3395471572876</v>
       </c>
       <c r="AI7" t="n">
-        <v>16.84111976623535</v>
+        <v>16.84111785888672</v>
       </c>
       <c r="AJ7" t="n">
-        <v>30.8597412109375</v>
+        <v>30.85973930358887</v>
       </c>
       <c r="AK7" t="n">
-        <v>5.183276176452637</v>
+        <v>5.18327522277832</v>
       </c>
       <c r="AL7" t="n">
-        <v>7.270424365997314</v>
+        <v>7.270422458648682</v>
       </c>
       <c r="AM7" t="n">
-        <v>9.358183860778809</v>
+        <v>9.358181953430176</v>
       </c>
       <c r="AN7" t="n">
-        <v>11.44404315948486</v>
+        <v>11.4440393447876</v>
       </c>
       <c r="AO7" t="n">
-        <v>13.52486038208008</v>
+        <v>13.52485752105713</v>
       </c>
       <c r="AP7" t="n">
-        <v>18.71195793151855</v>
+        <v>18.71195602416992</v>
       </c>
       <c r="AQ7" t="n">
         <v>23.85534858703613</v>
@@ -1340,127 +1340,127 @@
         </is>
       </c>
       <c r="C8" t="n">
-        <v>4.029058052710864</v>
+        <v>4.02905663251616</v>
       </c>
       <c r="D8" t="n">
-        <v>3.725793403258512</v>
+        <v>3.725792763344879</v>
       </c>
       <c r="E8" t="n">
-        <v>3.698896695630287</v>
+        <v>3.698895434473926</v>
       </c>
       <c r="F8" t="n">
-        <v>3.912491660035065</v>
+        <v>3.912490985588267</v>
       </c>
       <c r="G8" t="n">
-        <v>4.594166490283458</v>
+        <v>4.594167572806388</v>
       </c>
       <c r="H8" t="n">
-        <v>5.572701614068047</v>
+        <v>5.572702556939634</v>
       </c>
       <c r="I8" t="n">
-        <v>6.715055115728917</v>
+        <v>6.715057405062921</v>
       </c>
       <c r="J8" t="n">
-        <v>9.878019676472857</v>
+        <v>9.878021927140972</v>
       </c>
       <c r="K8" t="n">
-        <v>13.17186450944866</v>
+        <v>13.17186830809952</v>
       </c>
       <c r="L8" t="n">
-        <v>25.94795210206762</v>
+        <v>25.94795510105875</v>
       </c>
       <c r="M8" t="n">
-        <v>3.940364726180874</v>
+        <v>3.940362318039853</v>
       </c>
       <c r="N8" t="n">
-        <v>3.874744184774276</v>
+        <v>3.874741573033274</v>
       </c>
       <c r="O8" t="n">
-        <v>3.834519836162064</v>
+        <v>3.834518158831814</v>
       </c>
       <c r="P8" t="n">
-        <v>3.820027332089901</v>
+        <v>3.82002592876174</v>
       </c>
       <c r="Q8" t="n">
-        <v>3.833651277190133</v>
+        <v>3.833648772348766</v>
       </c>
       <c r="R8" t="n">
-        <v>3.984244764722769</v>
+        <v>3.984242446216209</v>
       </c>
       <c r="S8" t="n">
-        <v>4.312977901505201</v>
+        <v>4.312976045749904</v>
       </c>
       <c r="T8" t="n">
-        <v>6.395233604213271</v>
+        <v>6.395232579211017</v>
       </c>
       <c r="U8" t="n">
-        <v>3.698896695630287</v>
+        <v>3.698895434473926</v>
       </c>
       <c r="V8" t="n">
-        <v>3.912014569646967</v>
+        <v>3.912014221665434</v>
       </c>
       <c r="W8" t="n">
-        <v>4.593665263064757</v>
+        <v>4.593666134477511</v>
       </c>
       <c r="X8" t="n">
-        <v>5.571447438396181</v>
+        <v>5.571448058137008</v>
       </c>
       <c r="Y8" t="n">
-        <v>6.712033862535144</v>
+        <v>6.712036126404337</v>
       </c>
       <c r="Z8" t="n">
-        <v>9.210131302073171</v>
+        <v>9.21013382380823</v>
       </c>
       <c r="AA8" t="n">
-        <v>13.08208605973445</v>
+        <v>13.08208785113301</v>
       </c>
       <c r="AB8" t="n">
-        <v>25.0377664084093</v>
+        <v>25.03777081996365</v>
       </c>
       <c r="AC8" t="n">
-        <v>5.101924959307543</v>
+        <v>5.1019236508365</v>
       </c>
       <c r="AD8" t="n">
-        <v>6.303757760888261</v>
+        <v>6.303755340301594</v>
       </c>
       <c r="AE8" t="n">
-        <v>7.574400814518242</v>
+        <v>7.574397289105773</v>
       </c>
       <c r="AF8" t="n">
-        <v>8.885382368611143</v>
+        <v>8.885378934028054</v>
       </c>
       <c r="AG8" t="n">
-        <v>10.22048683455215</v>
+        <v>10.22048646131188</v>
       </c>
       <c r="AH8" t="n">
-        <v>13.62123601875802</v>
+        <v>13.62123377831666</v>
       </c>
       <c r="AI8" t="n">
-        <v>17.06764763953327</v>
+        <v>17.0676449574782</v>
       </c>
       <c r="AJ8" t="n">
         <v>31.01284130297632</v>
       </c>
       <c r="AK8" t="n">
-        <v>5.777545793880878</v>
+        <v>5.777544473355576</v>
       </c>
       <c r="AL8" t="n">
-        <v>7.698257734686349</v>
+        <v>7.698255504812945</v>
       </c>
       <c r="AM8" t="n">
-        <v>9.68958993333422</v>
+        <v>9.689586390121153</v>
       </c>
       <c r="AN8" t="n">
-        <v>11.71356525930446</v>
+        <v>11.71356200265483</v>
       </c>
       <c r="AO8" t="n">
-        <v>13.75224646510213</v>
+        <v>13.75224535555325</v>
       </c>
       <c r="AP8" t="n">
         <v>18.87916286616925</v>
       </c>
       <c r="AQ8" t="n">
-        <v>23.99476948008344</v>
+        <v>23.99476820824047</v>
       </c>
       <c r="AR8" t="n">
         <v>44.02345898956884</v>
@@ -1474,22 +1474,22 @@
         </is>
       </c>
       <c r="C9" t="n">
-        <v>0.9997962117195129</v>
+        <v>0.9997963309288025</v>
       </c>
       <c r="D9" t="n">
-        <v>0.9998556971549988</v>
+        <v>0.9998555779457092</v>
       </c>
       <c r="E9" t="n">
-        <v>0.9997830390930176</v>
+        <v>0.9997831583023071</v>
       </c>
       <c r="F9" t="n">
-        <v>0.9997265338897705</v>
+        <v>0.9997265934944153</v>
       </c>
       <c r="G9" t="n">
         <v>0.9996275305747986</v>
       </c>
       <c r="H9" t="n">
-        <v>0.9994871020317078</v>
+        <v>0.9994872212409973</v>
       </c>
       <c r="I9" t="n">
         <v>0.9993069171905518</v>
@@ -1498,106 +1498,106 @@
         <v>0.9986903071403503</v>
       </c>
       <c r="K9" t="n">
-        <v>0.997846245765686</v>
+        <v>0.9978463649749756</v>
       </c>
       <c r="L9" t="n">
-        <v>0.9925112128257751</v>
+        <v>0.9925113916397095</v>
       </c>
       <c r="M9" t="n">
-        <v>0.999799907207489</v>
+        <v>0.9997999668121338</v>
       </c>
       <c r="N9" t="n">
-        <v>0.9998007416725159</v>
+        <v>0.9998008608818054</v>
       </c>
       <c r="O9" t="n">
-        <v>0.999798595905304</v>
+        <v>0.9997988343238831</v>
       </c>
       <c r="P9" t="n">
         <v>0.9997933506965637</v>
       </c>
       <c r="Q9" t="n">
-        <v>0.9997851252555847</v>
+        <v>0.9997852444648743</v>
       </c>
       <c r="R9" t="n">
-        <v>0.9997509717941284</v>
+        <v>0.9997509121894836</v>
       </c>
       <c r="S9" t="n">
-        <v>0.9996943473815918</v>
+        <v>0.9996944665908813</v>
       </c>
       <c r="T9" t="n">
-        <v>0.9993012547492981</v>
+        <v>0.9993014931678772</v>
       </c>
       <c r="U9" t="n">
-        <v>0.9997830390930176</v>
+        <v>0.9997831583023071</v>
       </c>
       <c r="V9" t="n">
-        <v>0.9997265934944153</v>
+        <v>0.9997267127037048</v>
       </c>
       <c r="W9" t="n">
         <v>0.9996275305747986</v>
       </c>
       <c r="X9" t="n">
-        <v>0.9994862079620361</v>
+        <v>0.9994863271713257</v>
       </c>
       <c r="Y9" t="n">
-        <v>0.9993047714233398</v>
+        <v>0.9993048906326294</v>
       </c>
       <c r="Z9" t="n">
         <v>0.9988256692886353</v>
       </c>
       <c r="AA9" t="n">
-        <v>0.9978228211402893</v>
+        <v>0.9978229403495789</v>
       </c>
       <c r="AB9" t="n">
-        <v>0.9923169612884521</v>
+        <v>0.9923171401023865</v>
       </c>
       <c r="AC9" t="n">
-        <v>0.999720573425293</v>
+        <v>0.9997208118438721</v>
       </c>
       <c r="AD9" t="n">
-        <v>0.999611496925354</v>
+        <v>0.9996113777160645</v>
       </c>
       <c r="AE9" t="n">
-        <v>0.9994671940803528</v>
+        <v>0.9994672536849976</v>
       </c>
       <c r="AF9" t="n">
-        <v>0.9992865920066833</v>
+        <v>0.9992868304252625</v>
       </c>
       <c r="AG9" t="n">
-        <v>0.9990692138671875</v>
+        <v>0.9990693330764771</v>
       </c>
       <c r="AH9" t="n">
-        <v>0.9983554482460022</v>
+        <v>0.9983556866645813</v>
       </c>
       <c r="AI9" t="n">
         <v>0.9973829388618469</v>
       </c>
       <c r="AJ9" t="n">
-        <v>0.9904274344444275</v>
+        <v>0.9904276728630066</v>
       </c>
       <c r="AK9" t="n">
         <v>0.9995970129966736</v>
       </c>
       <c r="AL9" t="n">
-        <v>0.9992784261703491</v>
+        <v>0.9992785453796387</v>
       </c>
       <c r="AM9" t="n">
-        <v>0.9988356828689575</v>
+        <v>0.998835563659668</v>
       </c>
       <c r="AN9" t="n">
         <v>0.9982652068138123</v>
       </c>
       <c r="AO9" t="n">
-        <v>0.9975646138191223</v>
+        <v>0.9975647330284119</v>
       </c>
       <c r="AP9" t="n">
-        <v>0.9952123165130615</v>
+        <v>0.9952123761177063</v>
       </c>
       <c r="AQ9" t="n">
-        <v>0.9919604659080505</v>
+        <v>0.9919605255126953</v>
       </c>
       <c r="AR9" t="n">
-        <v>0.9692875146865845</v>
+        <v>0.969287633895874</v>
       </c>
     </row>
     <row r="10">
@@ -1612,85 +1612,85 @@
         </is>
       </c>
       <c r="C10" t="n">
-        <v>2.520872354507446</v>
+        <v>2.520873069763184</v>
       </c>
       <c r="D10" t="n">
-        <v>2.049843549728394</v>
+        <v>2.049844026565552</v>
       </c>
       <c r="E10" t="n">
-        <v>2.49658744985407</v>
+        <v>2.496588403528387</v>
       </c>
       <c r="F10" t="n">
-        <v>2.483515956185081</v>
+        <v>2.483518080277876</v>
       </c>
       <c r="G10" t="n">
-        <v>2.482743696732955</v>
+        <v>2.482745040546764</v>
       </c>
       <c r="H10" t="n">
-        <v>2.492159886793657</v>
+        <v>2.492159973491322</v>
       </c>
       <c r="I10" t="n">
-        <v>2.51182426105846</v>
+        <v>2.511824737895619</v>
       </c>
       <c r="J10" t="n">
         <v>2.597134590148926</v>
       </c>
       <c r="K10" t="n">
-        <v>2.782300038771196</v>
+        <v>2.782299995422363</v>
       </c>
       <c r="L10" t="n">
-        <v>4.292748234488747</v>
+        <v>4.292747670953924</v>
       </c>
       <c r="M10" t="n">
-        <v>2.543913971294056</v>
+        <v>2.54391301761974</v>
       </c>
       <c r="N10" t="n">
-        <v>3.054389346729625</v>
+        <v>3.054388089613481</v>
       </c>
       <c r="O10" t="n">
-        <v>3.946415641091086</v>
+        <v>3.946414210579612</v>
       </c>
       <c r="P10" t="n">
-        <v>5.040107293562456</v>
+        <v>5.040105733004483</v>
       </c>
       <c r="Q10" t="n">
-        <v>6.217551491477272</v>
+        <v>6.21754958412864</v>
       </c>
       <c r="R10" t="n">
-        <v>9.253607403148305</v>
+        <v>9.253605950962413</v>
       </c>
       <c r="S10" t="n">
-        <v>12.25272902575406</v>
+        <v>12.2527274868705</v>
       </c>
       <c r="T10" t="n">
-        <v>23.08312927592884</v>
+        <v>23.08312804048711</v>
       </c>
       <c r="U10" t="n">
-        <v>2.49658744985407</v>
+        <v>2.496588403528387</v>
       </c>
       <c r="V10" t="n">
-        <v>2.484747019681063</v>
+        <v>2.48474797335538</v>
       </c>
       <c r="W10" t="n">
-        <v>2.48504504290494</v>
+        <v>2.485045216300271</v>
       </c>
       <c r="X10" t="n">
-        <v>2.495169162750244</v>
+        <v>2.495169856331565</v>
       </c>
       <c r="Y10" t="n">
-        <v>2.514168826016513</v>
+        <v>2.514168392528187</v>
       </c>
       <c r="Z10" t="n">
-        <v>2.572210788726807</v>
+        <v>2.572210398587313</v>
       </c>
       <c r="AA10" t="n">
-        <v>2.764297398653897</v>
+        <v>2.764297138560902</v>
       </c>
       <c r="AB10" t="n">
-        <v>4.26233714277094</v>
+        <v>4.262336926026777</v>
       </c>
       <c r="AC10" t="n">
-        <v>3.633978843688965</v>
+        <v>3.633979558944702</v>
       </c>
       <c r="AD10" t="n">
         <v>4.897596836090088</v>
@@ -1699,13 +1699,13 @@
         <v>6.166963577270508</v>
       </c>
       <c r="AF10" t="n">
-        <v>7.436436176300049</v>
+        <v>7.436436653137207</v>
       </c>
       <c r="AG10" t="n">
-        <v>8.704400062561035</v>
+        <v>8.704401016235352</v>
       </c>
       <c r="AH10" t="n">
-        <v>11.87054443359375</v>
+        <v>11.87054538726807</v>
       </c>
       <c r="AI10" t="n">
         <v>15.02926540374756</v>
@@ -1717,7 +1717,7 @@
         <v>3.918492078781128</v>
       </c>
       <c r="AL10" t="n">
-        <v>5.31655740737915</v>
+        <v>5.316558837890625</v>
       </c>
       <c r="AM10" t="n">
         <v>6.714910507202148</v>
@@ -1746,85 +1746,85 @@
         </is>
       </c>
       <c r="C11" t="n">
-        <v>3.424288660511168</v>
+        <v>3.42428977452258</v>
       </c>
       <c r="D11" t="n">
         <v>3.003694008421635</v>
       </c>
       <c r="E11" t="n">
-        <v>3.410195274756314</v>
+        <v>3.410195152416859</v>
       </c>
       <c r="F11" t="n">
-        <v>3.405196440099795</v>
+        <v>3.405197395506765</v>
       </c>
       <c r="G11" t="n">
-        <v>3.410499572081692</v>
+        <v>3.410499972016955</v>
       </c>
       <c r="H11" t="n">
-        <v>3.426582557608007</v>
+        <v>3.426583186962782</v>
       </c>
       <c r="I11" t="n">
-        <v>3.455580735911509</v>
+        <v>3.455581742850374</v>
       </c>
       <c r="J11" t="n">
-        <v>3.57889429375599</v>
+        <v>3.578894934000896</v>
       </c>
       <c r="K11" t="n">
-        <v>3.805456591779543</v>
+        <v>3.805456587855378</v>
       </c>
       <c r="L11" t="n">
-        <v>5.550075913679242</v>
+        <v>5.550075538747111</v>
       </c>
       <c r="M11" t="n">
-        <v>3.49175774720743</v>
+        <v>3.49175711968296</v>
       </c>
       <c r="N11" t="n">
-        <v>4.011473200599034</v>
+        <v>4.011472614874183</v>
       </c>
       <c r="O11" t="n">
-        <v>4.838045289739028</v>
+        <v>4.838043913141372</v>
       </c>
       <c r="P11" t="n">
-        <v>5.839890777589154</v>
+        <v>5.839888852922739</v>
       </c>
       <c r="Q11" t="n">
-        <v>6.936764679583433</v>
+        <v>6.936762848995278</v>
       </c>
       <c r="R11" t="n">
-        <v>9.854700022224687</v>
+        <v>9.854698087155601</v>
       </c>
       <c r="S11" t="n">
-        <v>12.82282641228334</v>
+        <v>12.82282505512609</v>
       </c>
       <c r="T11" t="n">
-        <v>24.07810399532953</v>
+        <v>24.07810230291859</v>
       </c>
       <c r="U11" t="n">
-        <v>3.410195274756314</v>
+        <v>3.410195152416859</v>
       </c>
       <c r="V11" t="n">
-        <v>3.406308900141495</v>
+        <v>3.406309155060417</v>
       </c>
       <c r="W11" t="n">
-        <v>3.412839290367633</v>
+        <v>3.412839268175722</v>
       </c>
       <c r="X11" t="n">
-        <v>3.429857839754073</v>
+        <v>3.429857890387811</v>
       </c>
       <c r="Y11" t="n">
-        <v>3.457322085102887</v>
+        <v>3.457321323354972</v>
       </c>
       <c r="Z11" t="n">
-        <v>3.538759739704592</v>
+        <v>3.538760006529646</v>
       </c>
       <c r="AA11" t="n">
-        <v>3.778444524995995</v>
+        <v>3.778444092848842</v>
       </c>
       <c r="AB11" t="n">
-        <v>5.591791482067423</v>
+        <v>5.59179101053111</v>
       </c>
       <c r="AC11" t="n">
-        <v>4.381979688101997</v>
+        <v>4.381980341008432</v>
       </c>
       <c r="AD11" t="n">
         <v>5.470330582136371</v>
@@ -1833,43 +1833,43 @@
         <v>6.62579657606042</v>
       </c>
       <c r="AF11" t="n">
-        <v>7.818173477055494</v>
+        <v>7.818173964982393</v>
       </c>
       <c r="AG11" t="n">
-        <v>9.031336166868353</v>
+        <v>9.031336589252939</v>
       </c>
       <c r="AH11" t="n">
-        <v>12.11588282789243</v>
+        <v>12.11588471699801</v>
       </c>
       <c r="AI11" t="n">
         <v>15.23540110727033</v>
       </c>
       <c r="AJ11" t="n">
-        <v>27.69109739609465</v>
+        <v>27.69109629402281</v>
       </c>
       <c r="AK11" t="n">
-        <v>4.544335773809201</v>
+        <v>4.544336193529187</v>
       </c>
       <c r="AL11" t="n">
-        <v>5.787912849218316</v>
+        <v>5.787913508298221</v>
       </c>
       <c r="AM11" t="n">
-        <v>7.09042455222609</v>
+        <v>7.09042482122953</v>
       </c>
       <c r="AN11" t="n">
         <v>8.423595585345323</v>
       </c>
       <c r="AO11" t="n">
-        <v>9.772585019775985</v>
+        <v>9.772584629429181</v>
       </c>
       <c r="AP11" t="n">
-        <v>13.18024899700483</v>
+        <v>13.18024957585538</v>
       </c>
       <c r="AQ11" t="n">
         <v>16.60066633610634</v>
       </c>
       <c r="AR11" t="n">
-        <v>29.99667950373841</v>
+        <v>29.9966805211036</v>
       </c>
     </row>
     <row r="12">
@@ -1880,7 +1880,7 @@
         </is>
       </c>
       <c r="C12" t="n">
-        <v>0.9997943043708801</v>
+        <v>0.9997943639755249</v>
       </c>
       <c r="D12" t="n">
         <v>0.9998663067817688</v>
@@ -1889,7 +1889,7 @@
         <v>0.9997950792312622</v>
       </c>
       <c r="F12" t="n">
-        <v>0.9997949004173279</v>
+        <v>0.9997950196266174</v>
       </c>
       <c r="G12" t="n">
         <v>0.9997937083244324</v>
@@ -1898,25 +1898,25 @@
         <v>0.999791145324707</v>
       </c>
       <c r="I12" t="n">
-        <v>0.9997870922088623</v>
+        <v>0.9997871518135071</v>
       </c>
       <c r="J12" t="n">
-        <v>0.9997708797454834</v>
+        <v>0.9997709989547729</v>
       </c>
       <c r="K12" t="n">
-        <v>0.9997407197952271</v>
+        <v>0.9997408390045166</v>
       </c>
       <c r="L12" t="n">
-        <v>0.9994630813598633</v>
+        <v>0.9994632601737976</v>
       </c>
       <c r="M12" t="n">
-        <v>0.999782919883728</v>
+        <v>0.9997828006744385</v>
       </c>
       <c r="N12" t="n">
-        <v>0.9997382760047913</v>
+        <v>0.9997385144233704</v>
       </c>
       <c r="O12" t="n">
-        <v>0.9996612668037415</v>
+        <v>0.9996611475944519</v>
       </c>
       <c r="P12" t="n">
         <v>0.9995523691177368</v>
@@ -1925,82 +1925,82 @@
         <v>0.9994126558303833</v>
       </c>
       <c r="R12" t="n">
-        <v>0.9989357590675354</v>
+        <v>0.9989359378814697</v>
       </c>
       <c r="S12" t="n">
-        <v>0.9982829689979553</v>
+        <v>0.9982830882072449</v>
       </c>
       <c r="T12" t="n">
-        <v>0.9941701292991638</v>
+        <v>0.9941702485084534</v>
       </c>
       <c r="U12" t="n">
         <v>0.9997950792312622</v>
       </c>
       <c r="V12" t="n">
-        <v>0.9997947216033936</v>
+        <v>0.9997947812080383</v>
       </c>
       <c r="W12" t="n">
-        <v>0.9997934103012085</v>
+        <v>0.999793529510498</v>
       </c>
       <c r="X12" t="n">
-        <v>0.9997909069061279</v>
+        <v>0.9997910261154175</v>
       </c>
       <c r="Y12" t="n">
-        <v>0.9997873306274414</v>
+        <v>0.999787449836731</v>
       </c>
       <c r="Z12" t="n">
-        <v>0.9997768998146057</v>
+        <v>0.99977707862854</v>
       </c>
       <c r="AA12" t="n">
         <v>0.9997474551200867</v>
       </c>
       <c r="AB12" t="n">
-        <v>0.9995130300521851</v>
+        <v>0.9995131492614746</v>
       </c>
       <c r="AC12" t="n">
-        <v>0.9996751546859741</v>
+        <v>0.9996752738952637</v>
       </c>
       <c r="AD12" t="n">
-        <v>0.9995073676109314</v>
+        <v>0.9995074272155762</v>
       </c>
       <c r="AE12" t="n">
-        <v>0.9992897510528564</v>
+        <v>0.999289870262146</v>
       </c>
       <c r="AF12" t="n">
         <v>0.9990218877792358</v>
       </c>
       <c r="AG12" t="n">
-        <v>0.9987037181854248</v>
+        <v>0.9987038373947144</v>
       </c>
       <c r="AH12" t="n">
-        <v>0.9976822733879089</v>
+        <v>0.9976821541786194</v>
       </c>
       <c r="AI12" t="n">
-        <v>0.9963296055793762</v>
+        <v>0.9963297247886658</v>
       </c>
       <c r="AJ12" t="n">
-        <v>0.9875659942626953</v>
+        <v>0.9875661134719849</v>
       </c>
       <c r="AK12" t="n">
-        <v>0.9996381998062134</v>
+        <v>0.9996383190155029</v>
       </c>
       <c r="AL12" t="n">
-        <v>0.9994125366210938</v>
+        <v>0.9994124174118042</v>
       </c>
       <c r="AM12" t="n">
-        <v>0.9991163015365601</v>
+        <v>0.9991164803504944</v>
       </c>
       <c r="AN12" t="n">
-        <v>0.998749852180481</v>
+        <v>0.9987500905990601</v>
       </c>
       <c r="AO12" t="n">
-        <v>0.9983136057853699</v>
+        <v>0.9983137249946594</v>
       </c>
       <c r="AP12" t="n">
-        <v>0.9969160556793213</v>
+        <v>0.9969161748886108</v>
       </c>
       <c r="AQ12" t="n">
-        <v>0.9950838685035706</v>
+        <v>0.9950839877128601</v>
       </c>
       <c r="AR12" t="n">
         <v>0.9837189912796021</v>

</xml_diff>